<commit_message>
add 7/23 phen and biomass, fix 6/16 biomass
</commit_message>
<xml_diff>
--- a/data-raw/phen/rd_20200717-phen.xlsx
+++ b/data-raw/phen/rd_20200717-phen.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gina Laptippytop\Documents\_git_pkgs\maRsden\data-raw\phen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A3F72A6-E000-406F-BA55-B246161CBC88}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B27A00C4-112C-4CDA-BB98-14158F05B097}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -480,7 +480,7 @@
   <dimension ref="A1:Q47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="24.9" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -589,7 +589,7 @@
     </row>
     <row r="7" spans="1:16" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10">
-        <v>43993</v>
+        <v>44029</v>
       </c>
       <c r="B7" s="11">
         <v>13</v>

</xml_diff>